<commit_message>
Explore more call options, including RegisterId from managed add-in
</commit_message>
<xml_diff>
--- a/Test/ThreadSafeTest.xlsx
+++ b/Test/ThreadSafeTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ExcelDna\TechnicalSupport\WellsFargo\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1DE9682-E0EA-4A14-95D8-F5C80D9C065D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629300E3-2624-49A9-AC10-75DE75DE9814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11625" yWindow="1440" windowWidth="15330" windowHeight="13275" xr2:uid="{EB28390A-4BFF-4101-ACA0-D27C39EF25B4}"/>
+    <workbookView xWindow="11910" yWindow="1500" windowWidth="15330" windowHeight="13275" xr2:uid="{EB28390A-4BFF-4101-ACA0-D27C39EF25B4}"/>
   </bookViews>
   <sheets>
     <sheet name="C Functions Direct" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,10 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -51,11 +52,55 @@
       </extLst>
     </bk>
   </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="4">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="3"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
+  <valueMetadata count="4">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1"/>
+    </bk>
+    <bk>
+      <rc t="2" v="2"/>
+    </bk>
+    <bk>
+      <rc t="2" v="3"/>
+    </bk>
+  </valueMetadata>
 </metadata>
 </file>
 
@@ -520,6 +565,86 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="4">
+  <rv s="0">
+    <v>0</v>
+    <v>8</v>
+    <v>2</v>
+    <v>1</v>
+  </rv>
+  <rv s="0">
+    <v>0</v>
+    <v>8</v>
+    <v>19</v>
+    <v>1</v>
+  </rv>
+  <rv s="0">
+    <v>0</v>
+    <v>8</v>
+    <v>14</v>
+    <v>1</v>
+  </rv>
+  <rv s="0">
+    <v>0</v>
+    <v>8</v>
+    <v>4</v>
+    <v>1</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_error">
+    <k n="colOffset" t="i"/>
+    <k n="errorType" t="i"/>
+    <k n="rwOffset" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+</rvStructures>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -841,14 +966,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31F3B350-2661-447D-9AAD-8D0DCC82D920}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.7109375" customWidth="1"/>
     <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.7109375" customWidth="1"/>
@@ -884,13 +1011,13 @@
       <c r="C2">
         <v>10</v>
       </c>
-      <c r="D2" t="e" cm="1">
-        <f t="array" aca="1" ref="D2" ca="1">ThreadSafeCFunction(C2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E2" t="e" cm="1">
-        <f t="array" aca="1" ref="E2" ca="1">ThreadInfoFunction()</f>
-        <v>#NAME?</v>
+      <c r="D2" cm="1">
+        <f t="array" ref="D2">_xll.ThreadSafeCFunction(C2)</f>
+        <v>35981.47722557505</v>
+      </c>
+      <c r="E2" t="str" cm="1">
+        <f t="array" ref="E2">_xll.ThreadInfoFunction()</f>
+        <v>Thread: 9276, Time: 50962578</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -906,9 +1033,9 @@
       <c r="C3">
         <v>25</v>
       </c>
-      <c r="D3" t="e" cm="1">
-        <f t="array" aca="1" ref="D3" ca="1">ThreadSafeCalc(C3)</f>
-        <v>#NAME?</v>
+      <c r="D3" cm="1">
+        <f t="array" ref="D3">_xll.ThreadSafeCalc(C3)</f>
+        <v>36600.8676482499</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -924,9 +1051,9 @@
       <c r="C4">
         <v>15</v>
       </c>
-      <c r="D4" t="e" cm="1">
-        <f t="array" aca="1" ref="D4" ca="1">ThreadSafeXLOPER(C4)</f>
-        <v>#NAME?</v>
+      <c r="D4" cm="1">
+        <f t="array" ref="D4">_xll.ThreadSafeXLOPER(C4)</f>
+        <v>36006</v>
       </c>
       <c r="F4" t="s">
         <v>14</v>
@@ -942,9 +1069,9 @@
       <c r="C5">
         <v>3</v>
       </c>
-      <c r="D5" t="e" cm="1">
-        <f t="array" aca="1" ref="D5" ca="1">AllocatedMemoryFunction(C5)</f>
-        <v>#NAME?</v>
+      <c r="D5" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="D5" ca="1">_xll.AllocatedMemoryFunction(C5)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="F5" t="s">
         <v>17</v>
@@ -960,9 +1087,9 @@
       <c r="C6">
         <v>20</v>
       </c>
-      <c r="D6" t="e" cm="1">
-        <f t="array" aca="1" ref="D6" ca="1">AllocatedMemoryFunction(C6)</f>
-        <v>#NAME?</v>
+      <c r="D6" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="D6" ca="1">_xll.AllocatedMemoryFunction(C6)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="F6" t="s">
         <v>19</v>
@@ -978,9 +1105,9 @@
       <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" t="e" cm="1">
-        <f t="array" aca="1" ref="D7" ca="1">ThreadInfoFunction()</f>
-        <v>#NAME?</v>
+      <c r="D7" t="str" cm="1">
+        <f t="array" ref="D7">_xll.ThreadInfoFunction()</f>
+        <v>Thread: 35976, Time: 50987875</v>
       </c>
       <c r="F7" t="s">
         <v>23</v>
@@ -996,9 +1123,9 @@
       <c r="C8">
         <v>-10</v>
       </c>
-      <c r="D8" t="e" cm="1">
-        <f t="array" aca="1" ref="D8" ca="1">ThreadSafeCalc(C8)</f>
-        <v>#NAME?</v>
+      <c r="D8" cm="1">
+        <f t="array" ref="D8">_xll.ThreadSafeCalc(C8)</f>
+        <v>36076.544021110887</v>
       </c>
       <c r="F8" t="s">
         <v>25</v>
@@ -1014,9 +1141,9 @@
       <c r="C9">
         <v>0</v>
       </c>
-      <c r="D9" t="e" cm="1">
-        <f t="array" aca="1" ref="D9" ca="1">ThreadSafeCalc(C9)</f>
-        <v>#NAME?</v>
+      <c r="D9" cm="1">
+        <f t="array" ref="D9">_xll.ThreadSafeCalc(C9)</f>
+        <v>35976</v>
       </c>
       <c r="F9" t="s">
         <v>27</v>
@@ -1032,9 +1159,9 @@
       <c r="C10">
         <v>50</v>
       </c>
-      <c r="D10" t="e" cm="1">
-        <f t="array" aca="1" ref="D10" ca="1">ThreadSafeCalc(C10)</f>
-        <v>#NAME?</v>
+      <c r="D10" cm="1">
+        <f t="array" ref="D10">_xll.ThreadSafeCalc(C10)</f>
+        <v>38475.737625146299</v>
       </c>
       <c r="F10" t="s">
         <v>29</v>
@@ -1050,9 +1177,9 @@
       <c r="C11">
         <v>51</v>
       </c>
-      <c r="D11" t="e" cm="1">
-        <f t="array" aca="1" ref="D11" ca="1">ThreadSafeCalc(C11)</f>
-        <v>#NAME?</v>
+      <c r="D11" cm="1">
+        <f t="array" ref="D11">_xll.ThreadSafeCalc(C11)</f>
+        <v>38577.670229175841</v>
       </c>
       <c r="F11" t="s">
         <v>29</v>
@@ -1068,9 +1195,9 @@
       <c r="C12">
         <v>52</v>
       </c>
-      <c r="D12" t="e" cm="1">
-        <f t="array" aca="1" ref="D12" ca="1">ThreadSafeCalc(C12)</f>
-        <v>#NAME?</v>
+      <c r="D12" cm="1">
+        <f t="array" ref="D12">_xll.ThreadSafeCalc(C12)</f>
+        <v>11980.986627592039</v>
       </c>
       <c r="F12" t="s">
         <v>29</v>
@@ -1086,9 +1213,9 @@
       <c r="C13">
         <v>53</v>
       </c>
-      <c r="D13" t="e" cm="1">
-        <f t="array" aca="1" ref="D13" ca="1">ThreadSafeCalc(C13)</f>
-        <v>#NAME?</v>
+      <c r="D13" cm="1">
+        <f t="array" ref="D13">_xll.ThreadSafeCalc(C13)</f>
+        <v>38785.39592515018</v>
       </c>
       <c r="F13" t="s">
         <v>29</v>
@@ -1104,9 +1231,9 @@
       <c r="C14">
         <v>54</v>
       </c>
-      <c r="D14" t="e" cm="1">
-        <f t="array" aca="1" ref="D14" ca="1">ThreadSafeCalc(C14)</f>
-        <v>#NAME?</v>
+      <c r="D14" cm="1">
+        <f t="array" ref="D14">_xll.ThreadSafeCalc(C14)</f>
+        <v>38891.441210951147</v>
       </c>
       <c r="F14" t="s">
         <v>29</v>
@@ -1122,9 +1249,9 @@
       <c r="C15">
         <v>55</v>
       </c>
-      <c r="D15" t="e" cm="1">
-        <f t="array" aca="1" ref="D15" ca="1">ThreadSafeCalc(C15)</f>
-        <v>#NAME?</v>
+      <c r="D15" cm="1">
+        <f t="array" ref="D15">_xll.ThreadSafeCalc(C15)</f>
+        <v>39000.000244826639</v>
       </c>
       <c r="F15" t="s">
         <v>29</v>
@@ -1140,9 +1267,9 @@
       <c r="C16">
         <v>56</v>
       </c>
-      <c r="D16" t="e" cm="1">
-        <f t="array" aca="1" ref="D16" ca="1">ThreadSafeCalc(C16)</f>
-        <v>#NAME?</v>
+      <c r="D16" cm="1">
+        <f t="array" ref="D16">_xll.ThreadSafeCalc(C16)</f>
+        <v>39111.478448997914</v>
       </c>
       <c r="F16" t="s">
         <v>29</v>
@@ -1158,9 +1285,9 @@
       <c r="C17">
         <v>57</v>
       </c>
-      <c r="D17" t="e" cm="1">
-        <f t="array" aca="1" ref="D17" ca="1">ThreadSafeCalc(C17)</f>
-        <v>#NAME?</v>
+      <c r="D17" cm="1">
+        <f t="array" ref="D17">_xll.ThreadSafeCalc(C17)</f>
+        <v>39225.436164755251</v>
       </c>
       <c r="F17" t="s">
         <v>29</v>
@@ -1176,9 +1303,9 @@
       <c r="C18">
         <v>58</v>
       </c>
-      <c r="D18" t="e" cm="1">
-        <f t="array" aca="1" ref="D18" ca="1">ThreadSafeCalc(C18)</f>
-        <v>#NAME?</v>
+      <c r="D18" cm="1">
+        <f t="array" ref="D18">_xll.ThreadSafeCalc(C18)</f>
+        <v>39340.992872648087</v>
       </c>
       <c r="F18" t="s">
         <v>29</v>
@@ -1194,9 +1321,9 @@
       <c r="C19">
         <v>59</v>
       </c>
-      <c r="D19" t="e" cm="1">
-        <f t="array" aca="1" ref="D19" ca="1">ThreadSafeCalc(C19)</f>
-        <v>#NAME?</v>
+      <c r="D19" cm="1">
+        <f t="array" ref="D19">_xll.ThreadSafeCalc(C19)</f>
+        <v>39457.636738007139</v>
       </c>
       <c r="F19" t="s">
         <v>29</v>
@@ -1212,9 +1339,9 @@
       <c r="C20">
         <v>10000</v>
       </c>
-      <c r="D20" t="e" cm="1">
-        <f t="array" aca="1" ref="D20" ca="1">ThreadSafeCalc(C20)</f>
-        <v>#NAME?</v>
+      <c r="D20" cm="1">
+        <f t="array" ref="D20">_xll.ThreadSafeCalc(C20)</f>
+        <v>100035975.69438562</v>
       </c>
       <c r="F20" t="s">
         <v>40</v>
@@ -1229,14 +1356,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515BF833-0E12-406F-BFA8-613ACE7F1D03}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.7109375" customWidth="1"/>
     <col min="6" max="6" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.7109375" customWidth="1"/>
@@ -1272,13 +1401,13 @@
       <c r="C2">
         <v>10</v>
       </c>
-      <c r="D2" t="e" cm="1">
-        <f t="array" aca="1" ref="D2" ca="1">csThreadSafeCFunction(C2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E2" t="e" cm="1">
-        <f t="array" aca="1" ref="E2" ca="1">csThreadInfoFunction()</f>
-        <v>#NAME?</v>
+      <c r="D2" cm="1">
+        <f t="array" ref="D2">_xll.csThreadSafeCFunction(C2)</f>
+        <v>31.477225575051662</v>
+      </c>
+      <c r="E2" t="str" cm="1">
+        <f t="array" ref="E2">_xll.csThreadInfoFunction()</f>
+        <v>C# Thread: 25, Time: 50962562</v>
       </c>
       <c r="F2" t="s">
         <v>43</v>
@@ -1294,9 +1423,9 @@
       <c r="C3">
         <v>25</v>
       </c>
-      <c r="D3" t="e" cm="1">
-        <f t="array" aca="1" ref="D3" ca="1">csThreadSafeCalc(C3)</f>
-        <v>#NAME?</v>
+      <c r="D3" cm="1">
+        <f t="array" ref="D3">_xll.csThreadSafeCalc(C3)</f>
+        <v>644.86764824990223</v>
       </c>
       <c r="F3" t="s">
         <v>46</v>
@@ -1312,9 +1441,9 @@
       <c r="C4">
         <v>15</v>
       </c>
-      <c r="D4" t="e" cm="1">
-        <f t="array" aca="1" ref="D4" ca="1">csThreadSafeXLOPER(C4)</f>
-        <v>#NAME?</v>
+      <c r="D4" cm="1">
+        <f t="array" ref="D4">_xll.csThreadSafeXLOPER(C4)</f>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
         <v>49</v>
@@ -1330,9 +1459,9 @@
       <c r="C5">
         <v>3</v>
       </c>
-      <c r="D5" t="e" cm="1">
-        <f t="array" aca="1" ref="D5" ca="1">csAllocatedMemoryFunction(C5)</f>
-        <v>#NAME?</v>
+      <c r="D5" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="D5" ca="1">_xll.csAllocatedMemoryFunction(C5)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="F5" t="s">
         <v>52</v>
@@ -1348,9 +1477,9 @@
       <c r="C6">
         <v>15</v>
       </c>
-      <c r="D6" t="e" cm="1">
-        <f t="array" aca="1" ref="D6" ca="1">csAllocatedMemoryFunction(C6)</f>
-        <v>#NAME?</v>
+      <c r="D6" t="e" cm="1" vm="3">
+        <f t="array" aca="1" ref="D6" ca="1">_xll.csAllocatedMemoryFunction(C6)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="F6" t="s">
         <v>54</v>
@@ -1366,9 +1495,9 @@
       <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" t="e" cm="1">
-        <f t="array" aca="1" ref="D7" ca="1">csThreadInfoFunction()</f>
-        <v>#NAME?</v>
+      <c r="D7" t="str" cm="1">
+        <f t="array" ref="D7">_xll.csThreadInfoFunction()</f>
+        <v>C# Thread: 17, Time: 50962546</v>
       </c>
       <c r="F7" t="s">
         <v>57</v>
@@ -1385,8 +1514,8 @@
         <v>10</v>
       </c>
       <c r="D8" t="e" cm="1">
-        <f t="array" aca="1" ref="D8" ca="1">csAdvancedTest(C7, 5)</f>
-        <v>#NAME?</v>
+        <f t="array" ref="D8">_xll.csAdvancedTest(C7, 5)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="F8" t="s">
         <v>60</v>
@@ -1402,9 +1531,9 @@
       <c r="C9">
         <v>-10</v>
       </c>
-      <c r="D9" t="e" cm="1">
-        <f t="array" aca="1" ref="D9" ca="1">csThreadSafeCalc(C9)</f>
-        <v>#NAME?</v>
+      <c r="D9" cm="1">
+        <f t="array" ref="D9">_xll.csThreadSafeCalc(C9)</f>
+        <v>116.54402111088937</v>
       </c>
       <c r="F9" t="s">
         <v>62</v>
@@ -1420,9 +1549,9 @@
       <c r="C10">
         <v>0</v>
       </c>
-      <c r="D10" t="e" cm="1">
-        <f t="array" aca="1" ref="D10" ca="1">csThreadSafeCalc(C10)</f>
-        <v>#NAME?</v>
+      <c r="D10" cm="1">
+        <f t="array" ref="D10">_xll.csThreadSafeCalc(C10)</f>
+        <v>28</v>
       </c>
       <c r="F10" t="s">
         <v>64</v>
@@ -1438,9 +1567,9 @@
       <c r="C11">
         <v>60</v>
       </c>
-      <c r="D11" t="e" cm="1">
-        <f t="array" aca="1" ref="D11" ca="1">csThreadSafeCalc(C11)</f>
-        <v>#NAME?</v>
+      <c r="D11" cm="1">
+        <f t="array" ref="D11">_xll.csThreadSafeCalc(C11)</f>
+        <v>3615.6951893788978</v>
       </c>
       <c r="F11" t="s">
         <v>66</v>
@@ -1456,9 +1585,9 @@
       <c r="C12">
         <v>61</v>
       </c>
-      <c r="D12" t="e" cm="1">
-        <f t="array" aca="1" ref="D12" ca="1">csThreadSafeCalc(C12)</f>
-        <v>#NAME?</v>
+      <c r="D12" cm="1">
+        <f t="array" ref="D12">_xll.csThreadSafeCalc(C12)</f>
+        <v>3736.0338822299918</v>
       </c>
       <c r="F12" t="s">
         <v>66</v>
@@ -1474,9 +1603,9 @@
       <c r="C13">
         <v>62</v>
       </c>
-      <c r="D13" t="e" cm="1">
-        <f t="array" aca="1" ref="D13" ca="1">csThreadSafeCalc(C13)</f>
-        <v>#NAME?</v>
+      <c r="D13" cm="1">
+        <f t="array" ref="D13">_xll.csThreadSafeCalc(C13)</f>
+        <v>3859.2608193033507</v>
       </c>
       <c r="F13" t="s">
         <v>66</v>
@@ -1492,9 +1621,9 @@
       <c r="C14">
         <v>63</v>
       </c>
-      <c r="D14" t="e" cm="1">
-        <f t="array" aca="1" ref="D14" ca="1">csThreadSafeCalc(C14)</f>
-        <v>#NAME?</v>
+      <c r="D14" cm="1">
+        <f t="array" ref="D14">_xll.csThreadSafeCalc(C14)</f>
+        <v>3985.1673557003028</v>
       </c>
       <c r="F14" t="s">
         <v>66</v>
@@ -1510,9 +1639,9 @@
       <c r="C15">
         <v>64</v>
       </c>
-      <c r="D15" t="e" cm="1">
-        <f t="array" aca="1" ref="D15" ca="1">csThreadSafeCalc(C15)</f>
-        <v>#NAME?</v>
+      <c r="D15" cm="1">
+        <f t="array" ref="D15">_xll.csThreadSafeCalc(C15)</f>
+        <v>4118.9200260381967</v>
       </c>
       <c r="F15" t="s">
         <v>66</v>
@@ -1528,9 +1657,9 @@
       <c r="C16">
         <v>65</v>
       </c>
-      <c r="D16" t="e" cm="1">
-        <f t="array" aca="1" ref="D16" ca="1">csThreadSafeCalc(C16)</f>
-        <v>#NAME?</v>
+      <c r="D16" cm="1">
+        <f t="array" ref="D16">_xll.csThreadSafeCalc(C16)</f>
+        <v>4241.8268286794901</v>
       </c>
       <c r="F16" t="s">
         <v>66</v>
@@ -1546,9 +1675,9 @@
       <c r="C17">
         <v>66</v>
       </c>
-      <c r="D17" t="e" cm="1">
-        <f t="array" aca="1" ref="D17" ca="1">csThreadSafeCalc(C17)</f>
-        <v>#NAME?</v>
+      <c r="D17" cm="1">
+        <f t="array" ref="D17">_xll.csThreadSafeCalc(C17)</f>
+        <v>4371.9734488459762</v>
       </c>
       <c r="F17" t="s">
         <v>66</v>
@@ -1564,9 +1693,9 @@
       <c r="C18">
         <v>67</v>
       </c>
-      <c r="D18" t="e" cm="1">
-        <f t="array" aca="1" ref="D18" ca="1">csThreadSafeCalc(C18)</f>
-        <v>#NAME?</v>
+      <c r="D18" cm="1">
+        <f t="array" ref="D18">_xll.csThreadSafeCalc(C18)</f>
+        <v>4504.1444800210247</v>
       </c>
       <c r="F18" t="s">
         <v>66</v>
@@ -1582,9 +1711,9 @@
       <c r="C19">
         <v>68</v>
       </c>
-      <c r="D19" t="e" cm="1">
-        <f t="array" aca="1" ref="D19" ca="1">csThreadSafeCalc(C19)</f>
-        <v>#NAME?</v>
+      <c r="D19" cm="1">
+        <f t="array" ref="D19">_xll.csThreadSafeCalc(C19)</f>
+        <v>4639.1020723193105</v>
       </c>
       <c r="F19" t="s">
         <v>66</v>
@@ -1600,9 +1729,9 @@
       <c r="C20">
         <v>69</v>
       </c>
-      <c r="D20" t="e" cm="1">
-        <f t="array" aca="1" ref="D20" ca="1">csThreadSafeCalc(C20)</f>
-        <v>#NAME?</v>
+      <c r="D20" cm="1">
+        <f t="array" ref="D20">_xll.csThreadSafeCalc(C20)</f>
+        <v>4776.8852151862166</v>
       </c>
       <c r="F20" t="s">
         <v>66</v>
@@ -1618,9 +1747,9 @@
       <c r="C21">
         <v>10000</v>
       </c>
-      <c r="D21" t="e" cm="1">
-        <f t="array" aca="1" ref="D21" ca="1">csThreadSafeCalc(C21)</f>
-        <v>#NAME?</v>
+      <c r="D21" cm="1">
+        <f t="array" ref="D21">_xll.csThreadSafeCalc(C21)</f>
+        <v>100000015.69438562</v>
       </c>
       <c r="F21" t="s">
         <v>77</v>
@@ -1637,7 +1766,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1687,13 +1816,13 @@
       <c r="D2" t="b">
         <v>0</v>
       </c>
-      <c r="E2" t="e" cm="1">
-        <f t="array" aca="1" ref="E2" ca="1">TestThreadSafeCFunction(C2, D2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F2" t="e" cm="1">
-        <f t="array" aca="1" ref="F2" ca="1">ThreadSafeCFunction(C2)</f>
-        <v>#NAME?</v>
+      <c r="E2" cm="1">
+        <f t="array" ref="E2">_xll.TestThreadSafeCFunction(C2, D2)</f>
+        <v>3171.7459666924146</v>
+      </c>
+      <c r="F2" cm="1">
+        <f t="array" ref="F2">_xll.ThreadSafeCFunction(C2)</f>
+        <v>27607.745966692415</v>
       </c>
       <c r="G2" t="s">
         <v>82</v>
@@ -1712,13 +1841,13 @@
       <c r="D3" t="b">
         <v>1</v>
       </c>
-      <c r="E3" t="e" cm="1">
-        <f t="array" aca="1" ref="E3" ca="1">TestThreadSafeCFunction(C3, D3)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F3" t="e" cm="1">
-        <f t="array" aca="1" ref="F3" ca="1">csThreadSafeCFunction(C3)</f>
-        <v>#NAME?</v>
+      <c r="E3" cm="1">
+        <f t="array" ref="E3">_xll.TestThreadSafeCFunction(C3, D3)</f>
+        <v>34.745966692414832</v>
+      </c>
+      <c r="F3" cm="1">
+        <f t="array" ref="F3">_xll.csThreadSafeCFunction(C3)</f>
+        <v>23.745966692414832</v>
       </c>
       <c r="G3" t="s">
         <v>84</v>
@@ -1737,13 +1866,13 @@
       <c r="D4" t="b">
         <v>0</v>
       </c>
-      <c r="E4" t="e" cm="1">
-        <f t="array" aca="1" ref="E4" ca="1">TestThreadSafeCalc(C4, D4)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F4" t="e" cm="1">
-        <f t="array" aca="1" ref="F4" ca="1">ThreadSafeCalc(C4)</f>
-        <v>#NAME?</v>
+      <c r="E4" cm="1">
+        <f t="array" ref="E4">_xll.TestThreadSafeCalc(C4, D4)</f>
+        <v>31499.011968375908</v>
+      </c>
+      <c r="F4" cm="1">
+        <f t="array" ref="F4">_xll.ThreadSafeCalc(C4)</f>
+        <v>21207.011968375908</v>
       </c>
       <c r="G4" t="s">
         <v>87</v>
@@ -1762,13 +1891,13 @@
       <c r="D5" t="b">
         <v>1</v>
       </c>
-      <c r="E5" t="e" cm="1">
-        <f t="array" aca="1" ref="E5" ca="1">TestThreadSafeCalc(C5, D5)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F5" t="e" cm="1">
-        <f t="array" aca="1" ref="F5" ca="1">csThreadSafeCalc(C5)</f>
-        <v>#NAME?</v>
+      <c r="E5" cm="1">
+        <f t="array" ref="E5">_xll.TestThreadSafeCalc(C5, D5)</f>
+        <v>918.01196837590714</v>
+      </c>
+      <c r="F5" cm="1">
+        <f t="array" ref="F5">_xll.csThreadSafeCalc(C5)</f>
+        <v>924.01196837590714</v>
       </c>
       <c r="G5" t="s">
         <v>89</v>
@@ -1787,13 +1916,13 @@
       <c r="D6" t="b">
         <v>0</v>
       </c>
-      <c r="E6" t="e" cm="1">
-        <f t="array" aca="1" ref="E6" ca="1">TestThreadSafeXLOPER(C6, D6)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F6" t="e" cm="1">
-        <f t="array" aca="1" ref="F6" ca="1">ThreadSafeXLOPER(C6)</f>
-        <v>#NAME?</v>
+      <c r="E6" cm="1">
+        <f t="array" ref="E6">_xll.TestThreadSafeXLOPER(C6, D6)</f>
+        <v>31556</v>
+      </c>
+      <c r="F6" cm="1">
+        <f t="array" ref="F6">_xll.ThreadSafeXLOPER(C6)</f>
+        <v>27680</v>
       </c>
       <c r="G6" t="s">
         <v>92</v>
@@ -1812,13 +1941,13 @@
       <c r="D7" t="b">
         <v>1</v>
       </c>
-      <c r="E7" t="e" cm="1">
-        <f t="array" aca="1" ref="E7" ca="1">TestThreadSafeXLOPER(C7, D7)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F7" t="e" cm="1">
-        <f t="array" aca="1" ref="F7" ca="1">csThreadSafeXLOPER(C7)</f>
-        <v>#NAME?</v>
+      <c r="E7" cm="1">
+        <f t="array" ref="E7">_xll.TestThreadSafeXLOPER(C7, D7)</f>
+        <v>97</v>
+      </c>
+      <c r="F7" cm="1">
+        <f t="array" ref="F7">_xll.csThreadSafeXLOPER(C7)</f>
+        <v>106</v>
       </c>
       <c r="G7" t="s">
         <v>94</v>
@@ -1837,13 +1966,13 @@
       <c r="D8" t="b">
         <v>0</v>
       </c>
-      <c r="E8" t="e" cm="1">
-        <f t="array" aca="1" ref="E8" ca="1">TestAllocatedMemoryFunction(C8, D8)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F8" t="e" cm="1">
-        <f t="array" aca="1" ref="F8" ca="1">AllocatedMemoryFunction(C8)</f>
-        <v>#NAME?</v>
+      <c r="E8" t="e" cm="1" vm="4">
+        <f t="array" aca="1" ref="E8" ca="1">_xll.TestAllocatedMemoryFunction(C8, D8)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F8" t="e" cm="1" vm="4">
+        <f t="array" aca="1" ref="F8" ca="1">_xll.AllocatedMemoryFunction(C8)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="G8" t="s">
         <v>97</v>
@@ -1862,13 +1991,13 @@
       <c r="D9" t="b">
         <v>1</v>
       </c>
-      <c r="E9" t="e" cm="1">
-        <f t="array" aca="1" ref="E9" ca="1">TestAllocatedMemoryFunction(C9, D9)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F9" t="e" cm="1">
-        <f t="array" aca="1" ref="F9" ca="1">csAllocatedMemoryFunction(C9)</f>
-        <v>#NAME?</v>
+      <c r="E9" t="e" cm="1" vm="4">
+        <f t="array" aca="1" ref="E9" ca="1">_xll.TestAllocatedMemoryFunction(C9, D9)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F9" t="e" cm="1" vm="4">
+        <f t="array" aca="1" ref="F9" ca="1">_xll.csAllocatedMemoryFunction(C9)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="G9" t="s">
         <v>52</v>
@@ -1887,13 +2016,13 @@
       <c r="D10" t="b">
         <v>0</v>
       </c>
-      <c r="E10" t="e" cm="1">
-        <f t="array" aca="1" ref="E10" ca="1">TestThreadInfoFunction(D10)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F10" t="e" cm="1">
-        <f t="array" aca="1" ref="F10" ca="1">ThreadInfoFunction()</f>
-        <v>#NAME?</v>
+      <c r="E10" t="str" cm="1">
+        <f t="array" ref="E10">_xll.TestThreadInfoFunction(D10)</f>
+        <v>Thread: 3164, Time: 50962546</v>
+      </c>
+      <c r="F10" t="str" cm="1">
+        <f t="array" ref="F10">_xll.ThreadInfoFunction()</f>
+        <v>Thread: 27600, Time: 50962546</v>
       </c>
       <c r="G10" t="s">
         <v>101</v>
@@ -1912,13 +2041,13 @@
       <c r="D11" t="b">
         <v>1</v>
       </c>
-      <c r="E11" t="e" cm="1">
-        <f t="array" aca="1" ref="E11" ca="1">TestThreadInfoFunction(D11)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F11" t="e" cm="1">
-        <f t="array" aca="1" ref="F11" ca="1">csThreadInfoFunction()</f>
-        <v>#NAME?</v>
+      <c r="E11" t="str" cm="1">
+        <f t="array" ref="E11">_xll.TestThreadInfoFunction(D11)</f>
+        <v>C# Thread: 27, Time: 50962546</v>
+      </c>
+      <c r="F11" t="str" cm="1">
+        <f t="array" ref="F11">_xll.csThreadInfoFunction()</f>
+        <v>C# Thread: 16, Time: 50962546</v>
       </c>
       <c r="G11" t="s">
         <v>103</v>
@@ -1937,9 +2066,9 @@
       <c r="D13" t="b">
         <v>0</v>
       </c>
-      <c r="E13" t="e" cm="1">
-        <f t="array" aca="1" ref="E13" ca="1">TestMultipleThreadSafeCalls(C13, D13)</f>
-        <v>#NAME?</v>
+      <c r="E13" t="str" cm="1">
+        <f t="array" ref="E13">_xll.TestMultipleThreadSafeCalls(C13, D13)</f>
+        <v>Managed Thread: 33, Calc: 33099.7376251463, XLOPER: 30700, Info: Thread: 30600, Time: 50962546</v>
       </c>
       <c r="G13" t="s">
         <v>106</v>
@@ -1958,9 +2087,9 @@
       <c r="D14" t="b">
         <v>1</v>
       </c>
-      <c r="E14" t="e" cm="1">
-        <f t="array" aca="1" ref="E14" ca="1">TestMultipleThreadSafeCalls(C14, D14)</f>
-        <v>#NAME?</v>
+      <c r="E14" t="str" cm="1">
+        <f t="array" ref="E14">_xll.TestMultipleThreadSafeCalls(C14, D14)</f>
+        <v>Managed Thread: 35, Calc: 2520.7376251463, XLOPER: 121, Info: C# Thread: 21, Time: 50962546</v>
       </c>
       <c r="G14" t="s">
         <v>108</v>
@@ -1979,9 +2108,9 @@
       <c r="D16" t="b">
         <v>0</v>
       </c>
-      <c r="E16" t="e" cm="1">
-        <f t="array" aca="1" ref="E16" ca="1">TestPerformance(C16, 10, D16)</f>
-        <v>#NAME?</v>
+      <c r="E16" t="str" cm="1">
+        <f t="array" ref="E16">_xll.TestPerformance(C16, 10, D16)</f>
+        <v>C - Iterations: 10, Last Result: 29529.8167426066, Time: 156.21ms</v>
       </c>
       <c r="G16" t="s">
         <v>111</v>
@@ -2000,9 +2129,9 @@
       <c r="D17" t="b">
         <v>1</v>
       </c>
-      <c r="E17" t="e" cm="1">
-        <f t="array" aca="1" ref="E17" ca="1">TestPerformance(C17, 10, D17)</f>
-        <v>#NAME?</v>
+      <c r="E17" t="str" cm="1">
+        <f t="array" ref="E17">_xll.TestPerformance(C17, 10, D17)</f>
+        <v>C# - Iterations: 10, Last Result: 11904.8167426066, Time: 156.21ms</v>
       </c>
       <c r="G17" t="s">
         <v>113</v>
@@ -2021,9 +2150,9 @@
       <c r="D18" t="b">
         <v>0</v>
       </c>
-      <c r="E18" t="e" cm="1">
-        <f t="array" aca="1" ref="E18" ca="1">TestPerformance(C18, 50, D18)</f>
-        <v>#NAME?</v>
+      <c r="E18" t="str" cm="1">
+        <f t="array" ref="E18">_xll.TestPerformance(C18, 50, D18)</f>
+        <v>C - Iterations: 50, Last Result: 50956.0253513519, Time: 802.17ms</v>
       </c>
       <c r="G18" t="s">
         <v>115</v>
@@ -2042,9 +2171,9 @@
       <c r="D19" t="b">
         <v>1</v>
       </c>
-      <c r="E19" t="e" cm="1">
-        <f t="array" aca="1" ref="E19" ca="1">TestPerformance(C19, 50, D19)</f>
-        <v>#NAME?</v>
+      <c r="E19" t="str" cm="1">
+        <f t="array" ref="E19">_xll.TestPerformance(C19, 50, D19)</f>
+        <v>C# - Iterations: 50, Last Result: 22222.0253513519, Time: 802.17ms</v>
       </c>
       <c r="G19" t="s">
         <v>117</v>
@@ -2063,9 +2192,9 @@
       <c r="D20" t="s">
         <v>22</v>
       </c>
-      <c r="E20" t="e" cm="1">
-        <f t="array" aca="1" ref="E20" ca="1">ComparePerformance(C20, 25)</f>
-        <v>#NAME?</v>
+      <c r="E20" t="str" cm="1">
+        <f t="array" ref="E20">_xll.ComparePerformance(C20, 25)</f>
+        <v>C: 393.14ms (43863.0043130131), C#: 409.04ms (15404.0043130131)</v>
       </c>
       <c r="G20" t="s">
         <v>120</v>
@@ -2084,9 +2213,9 @@
       <c r="D22" t="b">
         <v>0</v>
       </c>
-      <c r="E22" t="e" cm="1">
-        <f t="array" aca="1" ref="E22" ca="1">TestThreadSafeCalc(C22, D22)</f>
-        <v>#NAME?</v>
+      <c r="E22" cm="1">
+        <f t="array" ref="E22">_xll.TestThreadSafeCalc(C22, D22)</f>
+        <v>69979.126702702779</v>
       </c>
       <c r="G22" t="s">
         <v>122</v>
@@ -2105,9 +2234,9 @@
       <c r="D23" t="b">
         <v>1</v>
       </c>
-      <c r="E23" t="e" cm="1">
-        <f t="array" aca="1" ref="E23" ca="1">TestThreadSafeCalc(C23, D23)</f>
-        <v>#NAME?</v>
+      <c r="E23" cm="1">
+        <f t="array" ref="E23">_xll.TestThreadSafeCalc(C23, D23)</f>
+        <v>40416.938109749281</v>
       </c>
       <c r="G23" t="s">
         <v>122</v>
@@ -2126,9 +2255,9 @@
       <c r="D24" t="b">
         <v>0</v>
       </c>
-      <c r="E24" t="e" cm="1">
-        <f t="array" aca="1" ref="E24" ca="1">TestThreadSafeCalc(C24, D24)</f>
-        <v>#NAME?</v>
+      <c r="E24" cm="1">
+        <f t="array" ref="E24">_xll.TestThreadSafeCalc(C24, D24)</f>
+        <v>66304.806418406864</v>
       </c>
       <c r="G24" t="s">
         <v>122</v>
@@ -2147,9 +2276,9 @@
       <c r="D25" t="b">
         <v>1</v>
       </c>
-      <c r="E25" t="e" cm="1">
-        <f t="array" aca="1" ref="E25" ca="1">TestThreadSafeCalc(C25, D25)</f>
-        <v>#NAME?</v>
+      <c r="E25" cm="1">
+        <f t="array" ref="E25">_xll.TestThreadSafeCalc(C25, D25)</f>
+        <v>41226.933309700165</v>
       </c>
       <c r="G25" t="s">
         <v>122</v>
@@ -2168,9 +2297,9 @@
       <c r="D26" t="b">
         <v>0</v>
       </c>
-      <c r="E26" t="e" cm="1">
-        <f t="array" aca="1" ref="E26" ca="1">TestThreadSafeCalc(C26, D26)</f>
-        <v>#NAME?</v>
+      <c r="E26" cm="1">
+        <f t="array" ref="E26">_xll.TestThreadSafeCalc(C26, D26)</f>
+        <v>44780.20212035931</v>
       </c>
       <c r="G26" t="s">
         <v>122</v>
@@ -2189,9 +2318,9 @@
       <c r="D27" t="b">
         <v>1</v>
       </c>
-      <c r="E27" t="e" cm="1">
-        <f t="array" aca="1" ref="E27" ca="1">TestThreadSafeCalc(C27, D27)</f>
-        <v>#NAME?</v>
+      <c r="E27" cm="1">
+        <f t="array" ref="E27">_xll.TestThreadSafeCalc(C27, D27)</f>
+        <v>42043.285102492235</v>
       </c>
       <c r="G27" t="s">
         <v>122</v>
@@ -2210,9 +2339,9 @@
       <c r="D28" t="b">
         <v>0</v>
       </c>
-      <c r="E28" t="e" cm="1">
-        <f t="array" aca="1" ref="E28" ca="1">TestThreadSafeCalc(C28, D28)</f>
-        <v>#NAME?</v>
+      <c r="E28" cm="1">
+        <f t="array" ref="E28">_xll.TestThreadSafeCalc(C28, D28)</f>
+        <v>51711.025358096871</v>
       </c>
       <c r="G28" t="s">
         <v>122</v>
@@ -2231,9 +2360,9 @@
       <c r="D29" t="b">
         <v>1</v>
       </c>
-      <c r="E29" t="e" cm="1">
-        <f t="array" aca="1" ref="E29" ca="1">TestThreadSafeCalc(C29, D29)</f>
-        <v>#NAME?</v>
+      <c r="E29" cm="1">
+        <f t="array" ref="E29">_xll.TestThreadSafeCalc(C29, D29)</f>
+        <v>42868.661694972456</v>
       </c>
       <c r="G29" t="s">
         <v>122</v>
@@ -2252,9 +2381,9 @@
       <c r="D30" t="b">
         <v>0</v>
       </c>
-      <c r="E30" t="e" cm="1">
-        <f t="array" aca="1" ref="E30" ca="1">TestThreadSafeCalc(C30, D30)</f>
-        <v>#NAME?</v>
+      <c r="E30" cm="1">
+        <f t="array" ref="E30">_xll.TestThreadSafeCalc(C30, D30)</f>
+        <v>44028.609067930192</v>
       </c>
       <c r="G30" t="s">
         <v>122</v>

</xml_diff>